<commit_message>
AI agent is hardcoded, robot turns left/right/straight at tuple recognition. Microtaur stops at dead end.
</commit_message>
<xml_diff>
--- a/TestData/SensorToWallCmMeasurements.xlsx
+++ b/TestData/SensorToWallCmMeasurements.xlsx
@@ -387,7 +387,7 @@
                   <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>167.33333333333334</c:v>
+                  <c:v>200.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>207.33333333333334</c:v>
@@ -487,11 +487,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="56742912"/>
-        <c:axId val="130854272"/>
+        <c:axId val="47054336"/>
+        <c:axId val="40268288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56742912"/>
+        <c:axId val="47054336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -524,7 +524,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130854272"/>
+        <c:crossAx val="40268288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -532,7 +532,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130854272"/>
+        <c:axId val="40268288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,7 +562,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56742912"/>
+        <c:crossAx val="47054336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +959,7 @@
         <v>683</v>
       </c>
       <c r="E3" s="5">
-        <f>AVERAGE(B3:D3)</f>
+        <f t="shared" ref="E3:E24" si="0">AVERAGE(B3:D3)</f>
         <v>694.66666666666663</v>
       </c>
     </row>
@@ -977,7 +977,7 @@
         <v>751</v>
       </c>
       <c r="E4" s="5">
-        <f>AVERAGE(B4:D4)</f>
+        <f t="shared" si="0"/>
         <v>753</v>
       </c>
     </row>
@@ -995,7 +995,7 @@
         <v>1009</v>
       </c>
       <c r="E5" s="5">
-        <f>AVERAGE(B5:D5)</f>
+        <f t="shared" si="0"/>
         <v>1008.6666666666666</v>
       </c>
     </row>
@@ -1013,7 +1013,7 @@
         <v>1011</v>
       </c>
       <c r="E6" s="5">
-        <f>AVERAGE(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>1009.6666666666666</v>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
         <v>949</v>
       </c>
       <c r="E7" s="5">
-        <f>AVERAGE(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>951</v>
       </c>
     </row>
@@ -1049,7 +1049,7 @@
         <v>885</v>
       </c>
       <c r="E8" s="5">
-        <f>AVERAGE(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>884.33333333333337</v>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
         <v>758</v>
       </c>
       <c r="E9" s="5">
-        <f>AVERAGE(B9:D9)</f>
+        <f t="shared" si="0"/>
         <v>757.66666666666663</v>
       </c>
     </row>
@@ -1085,7 +1085,7 @@
         <v>637</v>
       </c>
       <c r="E10" s="5">
-        <f>AVERAGE(B10:D10)</f>
+        <f t="shared" si="0"/>
         <v>636.33333333333337</v>
       </c>
     </row>
@@ -1103,7 +1103,7 @@
         <v>564</v>
       </c>
       <c r="E11" s="5">
-        <f>AVERAGE(B11:D11)</f>
+        <f t="shared" si="0"/>
         <v>566</v>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
         <v>499</v>
       </c>
       <c r="E12" s="5">
-        <f>AVERAGE(B12:D12)</f>
+        <f t="shared" si="0"/>
         <v>499.66666666666669</v>
       </c>
     </row>
@@ -1139,7 +1139,7 @@
         <v>452</v>
       </c>
       <c r="E13" s="5">
-        <f>AVERAGE(B13:D13)</f>
+        <f t="shared" si="0"/>
         <v>448.33333333333331</v>
       </c>
     </row>
@@ -1157,7 +1157,7 @@
         <v>393</v>
       </c>
       <c r="E14" s="5">
-        <f>AVERAGE(B14:D14)</f>
+        <f t="shared" si="0"/>
         <v>396.33333333333331</v>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
         <v>361</v>
       </c>
       <c r="E15" s="5">
-        <f>AVERAGE(B15:D15)</f>
+        <f t="shared" si="0"/>
         <v>360.66666666666669</v>
       </c>
     </row>
@@ -1193,7 +1193,7 @@
         <v>310</v>
       </c>
       <c r="E16" s="6">
-        <f>AVERAGE(B16:D16)</f>
+        <f t="shared" si="0"/>
         <v>311.66666666666669</v>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
         <v>311</v>
       </c>
       <c r="E17" s="6">
-        <f>AVERAGE(B17:D17)</f>
+        <f t="shared" si="0"/>
         <v>312</v>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
         <v>267</v>
       </c>
       <c r="E18" s="5">
-        <f>AVERAGE(B18:D18)</f>
+        <f t="shared" si="0"/>
         <v>268.66666666666669</v>
       </c>
     </row>
@@ -1247,7 +1247,7 @@
         <v>268</v>
       </c>
       <c r="E19" s="5">
-        <f>AVERAGE(B19:D19)</f>
+        <f t="shared" si="0"/>
         <v>268</v>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
         <v>235</v>
       </c>
       <c r="E20" s="5">
-        <f>AVERAGE(B20:D20)</f>
+        <f t="shared" si="0"/>
         <v>237.66666666666666</v>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
         <v>218</v>
       </c>
       <c r="E21" s="5">
-        <f>AVERAGE(B21:D21)</f>
+        <f t="shared" si="0"/>
         <v>218.66666666666666</v>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
         <v>202</v>
       </c>
       <c r="E22" s="5">
-        <f>AVERAGE(B22:D22)</f>
+        <f t="shared" si="0"/>
         <v>199</v>
       </c>
     </row>
@@ -1319,7 +1319,7 @@
         <v>190</v>
       </c>
       <c r="E23" s="5">
-        <f>AVERAGE(B23:D23)</f>
+        <f t="shared" si="0"/>
         <v>189</v>
       </c>
     </row>
@@ -1337,7 +1337,7 @@
         <v>178</v>
       </c>
       <c r="E24" s="5">
-        <f>AVERAGE(B24:D24)</f>
+        <f t="shared" si="0"/>
         <v>179</v>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
         <v>806</v>
       </c>
       <c r="E28" s="5">
-        <f>AVERAGE(B28:D28)</f>
+        <f t="shared" ref="E28:E47" si="1">AVERAGE(B28:D28)</f>
         <v>805.33333333333337</v>
       </c>
     </row>
@@ -1399,7 +1399,7 @@
         <v>999</v>
       </c>
       <c r="E29" s="5">
-        <f>AVERAGE(B29:D29)</f>
+        <f t="shared" si="1"/>
         <v>1002</v>
       </c>
       <c r="G29" s="3"/>
@@ -1420,7 +1420,7 @@
         <v>1011</v>
       </c>
       <c r="E30" s="5">
-        <f>AVERAGE(B30:D30)</f>
+        <f t="shared" si="1"/>
         <v>1011.3333333333334</v>
       </c>
       <c r="G30" s="3"/>
@@ -1441,7 +1441,7 @@
         <v>875</v>
       </c>
       <c r="E31" s="5">
-        <f>AVERAGE(B31:D31)</f>
+        <f t="shared" si="1"/>
         <v>874.66666666666663</v>
       </c>
       <c r="F31" s="3">
@@ -1462,7 +1462,7 @@
         <v>734</v>
       </c>
       <c r="E32" s="5">
-        <f>AVERAGE(B32:D32)</f>
+        <f t="shared" si="1"/>
         <v>737</v>
       </c>
     </row>
@@ -1480,7 +1480,7 @@
         <v>635</v>
       </c>
       <c r="E33" s="5">
-        <f>AVERAGE(B33:D33)</f>
+        <f t="shared" si="1"/>
         <v>635.33333333333337</v>
       </c>
     </row>
@@ -1498,7 +1498,7 @@
         <v>557</v>
       </c>
       <c r="E34" s="5">
-        <f>AVERAGE(B34:D34)</f>
+        <f t="shared" si="1"/>
         <v>557.33333333333337</v>
       </c>
     </row>
@@ -1516,7 +1516,7 @@
         <v>492</v>
       </c>
       <c r="E35" s="5">
-        <f>AVERAGE(B35:D35)</f>
+        <f t="shared" si="1"/>
         <v>492</v>
       </c>
     </row>
@@ -1534,7 +1534,7 @@
         <v>443</v>
       </c>
       <c r="E36" s="5">
-        <f>AVERAGE(B36:D36)</f>
+        <f t="shared" si="1"/>
         <v>444.66666666666669</v>
       </c>
     </row>
@@ -1552,7 +1552,7 @@
         <v>401</v>
       </c>
       <c r="E37" s="5">
-        <f>AVERAGE(B37:D37)</f>
+        <f t="shared" si="1"/>
         <v>403</v>
       </c>
     </row>
@@ -1570,7 +1570,7 @@
         <v>372</v>
       </c>
       <c r="E38" s="5">
-        <f>AVERAGE(B38:D38)</f>
+        <f t="shared" si="1"/>
         <v>371.33333333333331</v>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
         <v>347</v>
       </c>
       <c r="E39" s="6">
-        <f>AVERAGE(B39:D39)</f>
+        <f t="shared" si="1"/>
         <v>345.66666666666669</v>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
         <v>324</v>
       </c>
       <c r="E40" s="6">
-        <f>AVERAGE(B40:D40)</f>
+        <f t="shared" si="1"/>
         <v>324.33333333333331</v>
       </c>
     </row>
@@ -1624,7 +1624,7 @@
         <v>306</v>
       </c>
       <c r="E41" s="5">
-        <f>AVERAGE(B41:D41)</f>
+        <f t="shared" si="1"/>
         <v>307</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
         <v>283</v>
       </c>
       <c r="E42" s="5">
-        <f>AVERAGE(B42:D42)</f>
+        <f t="shared" si="1"/>
         <v>284.66666666666669</v>
       </c>
     </row>
@@ -1660,7 +1660,7 @@
         <v>262</v>
       </c>
       <c r="E43" s="5">
-        <f>AVERAGE(B43:D43)</f>
+        <f t="shared" si="1"/>
         <v>262</v>
       </c>
     </row>
@@ -1678,7 +1678,7 @@
         <v>233</v>
       </c>
       <c r="E44" s="5">
-        <f>AVERAGE(B44:D44)</f>
+        <f t="shared" si="1"/>
         <v>237</v>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
         <v>218</v>
       </c>
       <c r="E45" s="5">
-        <f>AVERAGE(B45:D45)</f>
+        <f t="shared" si="1"/>
         <v>215</v>
       </c>
     </row>
@@ -1708,14 +1708,14 @@
         <v>204</v>
       </c>
       <c r="C46" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D46" s="3">
         <v>198</v>
       </c>
       <c r="E46" s="5">
-        <f>AVERAGE(B46:D46)</f>
-        <v>167.33333333333334</v>
+        <f t="shared" si="1"/>
+        <v>200.66666666666666</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1732,7 +1732,7 @@
         <v>206</v>
       </c>
       <c r="E47" s="5">
-        <f>AVERAGE(B47:D47)</f>
+        <f t="shared" si="1"/>
         <v>207.33333333333334</v>
       </c>
     </row>
@@ -1776,7 +1776,7 @@
         <v>775</v>
       </c>
       <c r="E51" s="5">
-        <f>AVERAGE(B51:D51)</f>
+        <f t="shared" ref="E51:E70" si="2">AVERAGE(B51:D51)</f>
         <v>777</v>
       </c>
     </row>
@@ -1794,7 +1794,7 @@
         <v>1001</v>
       </c>
       <c r="E52" s="5">
-        <f>AVERAGE(B52:D52)</f>
+        <f t="shared" si="2"/>
         <v>1001.6666666666666</v>
       </c>
     </row>
@@ -1812,7 +1812,7 @@
         <v>993</v>
       </c>
       <c r="E53" s="5">
-        <f>AVERAGE(B53:D53)</f>
+        <f t="shared" si="2"/>
         <v>993.66666666666663</v>
       </c>
     </row>
@@ -1830,7 +1830,7 @@
         <v>849</v>
       </c>
       <c r="E54" s="5">
-        <f>AVERAGE(B54:D54)</f>
+        <f t="shared" si="2"/>
         <v>850.33333333333337</v>
       </c>
     </row>
@@ -1848,7 +1848,7 @@
         <v>714</v>
       </c>
       <c r="E55" s="5">
-        <f>AVERAGE(B55:D55)</f>
+        <f t="shared" si="2"/>
         <v>712.66666666666663</v>
       </c>
     </row>
@@ -1866,7 +1866,7 @@
         <v>622</v>
       </c>
       <c r="E56" s="5">
-        <f>AVERAGE(B56:D56)</f>
+        <f t="shared" si="2"/>
         <v>623</v>
       </c>
       <c r="F56" s="5"/>
@@ -1885,7 +1885,7 @@
         <v>541</v>
       </c>
       <c r="E57" s="5">
-        <f>AVERAGE(B57:D57)</f>
+        <f t="shared" si="2"/>
         <v>540.66666666666663</v>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
         <v>478</v>
       </c>
       <c r="E58" s="5">
-        <f>AVERAGE(B58:D58)</f>
+        <f t="shared" si="2"/>
         <v>480.33333333333331</v>
       </c>
     </row>
@@ -1921,7 +1921,7 @@
         <v>430</v>
       </c>
       <c r="E59" s="5">
-        <f>AVERAGE(B59:D59)</f>
+        <f t="shared" si="2"/>
         <v>431.66666666666669</v>
       </c>
     </row>
@@ -1939,7 +1939,7 @@
         <v>387</v>
       </c>
       <c r="E60" s="5">
-        <f>AVERAGE(B60:D60)</f>
+        <f t="shared" si="2"/>
         <v>390.66666666666669</v>
       </c>
     </row>
@@ -1957,7 +1957,7 @@
         <v>357</v>
       </c>
       <c r="E61" s="5">
-        <f>AVERAGE(B61:D61)</f>
+        <f t="shared" si="2"/>
         <v>357.66666666666669</v>
       </c>
     </row>
@@ -1975,7 +1975,7 @@
         <v>323</v>
       </c>
       <c r="E62" s="6">
-        <f>AVERAGE(B62:D62)</f>
+        <f t="shared" si="2"/>
         <v>322.33333333333331</v>
       </c>
     </row>
@@ -1993,7 +1993,7 @@
         <v>304</v>
       </c>
       <c r="E63" s="6">
-        <f>AVERAGE(B63:D63)</f>
+        <f t="shared" si="2"/>
         <v>302.66666666666669</v>
       </c>
     </row>
@@ -2011,7 +2011,7 @@
         <v>276</v>
       </c>
       <c r="E64" s="5">
-        <f>AVERAGE(B64:D64)</f>
+        <f t="shared" si="2"/>
         <v>278.66666666666669</v>
       </c>
     </row>
@@ -2029,7 +2029,7 @@
         <v>260</v>
       </c>
       <c r="E65" s="5">
-        <f>AVERAGE(B65:D65)</f>
+        <f t="shared" si="2"/>
         <v>260.33333333333331</v>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
         <v>246</v>
       </c>
       <c r="E66" s="5">
-        <f>AVERAGE(B66:D66)</f>
+        <f t="shared" si="2"/>
         <v>248.66666666666666</v>
       </c>
     </row>
@@ -2065,7 +2065,7 @@
         <v>231</v>
       </c>
       <c r="E67" s="5">
-        <f>AVERAGE(B67:D67)</f>
+        <f t="shared" si="2"/>
         <v>234.33333333333334</v>
       </c>
     </row>
@@ -2083,7 +2083,7 @@
         <v>209</v>
       </c>
       <c r="E68" s="5">
-        <f>AVERAGE(B68:D68)</f>
+        <f t="shared" si="2"/>
         <v>209.66666666666666</v>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
         <v>194</v>
       </c>
       <c r="E69" s="5">
-        <f>AVERAGE(B69:D69)</f>
+        <f t="shared" si="2"/>
         <v>186</v>
       </c>
     </row>
@@ -2119,7 +2119,7 @@
         <v>188</v>
       </c>
       <c r="E70" s="5">
-        <f>AVERAGE(B70:D70)</f>
+        <f t="shared" si="2"/>
         <v>190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added rudimentary error correcting code for distances greater than 1 unit. Difficult to tell the effectiveness of error correcting code because of wheel hardware issue. Still need to make code more concise.
</commit_message>
<xml_diff>
--- a/TestData/SensorToWallCmMeasurements.xlsx
+++ b/TestData/SensorToWallCmMeasurements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Sensor to Wall (cm)</t>
   </si>
@@ -40,6 +40,21 @@
   </si>
   <si>
     <t>RIGHT IR SENSOR</t>
+  </si>
+  <si>
+    <t>Robot in Middle of Unit</t>
+  </si>
+  <si>
+    <t>Left Sensor</t>
+  </si>
+  <si>
+    <t>Right Sensor</t>
+  </si>
+  <si>
+    <t>STDEV</t>
+  </si>
+  <si>
+    <t>CM</t>
   </si>
 </sst>
 </file>
@@ -83,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -96,6 +111,15 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -487,11 +511,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="47054336"/>
-        <c:axId val="40268288"/>
+        <c:axId val="48455168"/>
+        <c:axId val="40201600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47054336"/>
+        <c:axId val="48455168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -524,7 +548,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40268288"/>
+        <c:crossAx val="40201600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -532,7 +556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40268288"/>
+        <c:axId val="40201600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,7 +586,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47054336"/>
+        <c:crossAx val="48455168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -906,16 +930,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="3"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="3"/>
     <col min="5" max="5" width="9.140625" style="5"/>
   </cols>
   <sheetData>
@@ -2121,6 +2146,129 @@
       <c r="E70" s="5">
         <f t="shared" si="2"/>
         <v>190</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>534</v>
+      </c>
+      <c r="B74" s="10">
+        <f>AVERAGE(A74:A79)</f>
+        <v>542.66666666666663</v>
+      </c>
+      <c r="C74" s="10">
+        <f>_xlfn.STDEV.P(A74:A79)</f>
+        <v>11.86966254317657</v>
+      </c>
+      <c r="D74" s="3">
+        <v>7.3479999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>531</v>
+      </c>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>540</v>
+      </c>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>551</v>
+      </c>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>535</v>
+      </c>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>565</v>
+      </c>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="9">
+        <v>409</v>
+      </c>
+      <c r="B82" s="10">
+        <f>AVERAGE(A82:A87)</f>
+        <v>426.5</v>
+      </c>
+      <c r="C82" s="10">
+        <f>_xlfn.STDEV.P(A82:A87)</f>
+        <v>15.88238017426859</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="9">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="9">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="9">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="9">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="9">
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tuple recognition is almost completed. Mouse recognizes when can go straight, and does not mess up on the next tuple. TODO next: Poll opposite of the sensor that triggered a tuple in goForward method.
</commit_message>
<xml_diff>
--- a/TestData/SensorToWallCmMeasurements.xlsx
+++ b/TestData/SensorToWallCmMeasurements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>Sensor to Wall (cm)</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>RIGHT IR SENSOR</t>
+  </si>
+  <si>
+    <t>FRONT IR SENSOR; After Weird Behavior</t>
   </si>
 </sst>
 </file>
@@ -83,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -95,6 +98,9 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,11 +493,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="47054336"/>
-        <c:axId val="40268288"/>
+        <c:axId val="144931840"/>
+        <c:axId val="75405504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47054336"/>
+        <c:axId val="144931840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -524,7 +530,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40268288"/>
+        <c:crossAx val="75405504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -532,7 +538,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40268288"/>
+        <c:axId val="75405504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,7 +568,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47054336"/>
+        <c:crossAx val="144931840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -588,16 +594,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>438149</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>138113</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -906,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,16 +925,23 @@
     <col min="5" max="5" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="G1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -944,8 +957,23 @@
       <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -962,8 +990,15 @@
         <f t="shared" ref="E3:E24" si="0">AVERAGE(B3:D3)</f>
         <v>694.66666666666663</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -980,8 +1015,15 @@
         <f t="shared" si="0"/>
         <v>753</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.5</v>
       </c>
@@ -998,8 +1040,15 @@
         <f t="shared" si="0"/>
         <v>1008.6666666666666</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>2.5</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1016,8 +1065,15 @@
         <f t="shared" si="0"/>
         <v>1009.6666666666666</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.5</v>
       </c>
@@ -1034,8 +1090,15 @@
         <f t="shared" si="0"/>
         <v>951</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>3.5</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1052,8 +1115,15 @@
         <f t="shared" si="0"/>
         <v>884.33333333333337</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1070,8 +1140,15 @@
         <f t="shared" si="0"/>
         <v>757.66666666666663</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1088,8 +1165,15 @@
         <f t="shared" si="0"/>
         <v>636.33333333333337</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1106,8 +1190,15 @@
         <f t="shared" si="0"/>
         <v>566</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1124,8 +1215,15 @@
         <f t="shared" si="0"/>
         <v>499.66666666666669</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>8</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1142,8 +1240,15 @@
         <f t="shared" si="0"/>
         <v>448.33333333333331</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>9</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1160,8 +1265,15 @@
         <f t="shared" si="0"/>
         <v>396.33333333333331</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1178,8 +1290,15 @@
         <f t="shared" si="0"/>
         <v>360.66666666666669</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>11</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1196,8 +1315,15 @@
         <f t="shared" si="0"/>
         <v>311.66666666666669</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>12</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1214,8 +1340,15 @@
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>13</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1232,8 +1365,15 @@
         <f t="shared" si="0"/>
         <v>268.66666666666669</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>14</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1250,8 +1390,15 @@
         <f t="shared" si="0"/>
         <v>268</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>15</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1268,8 +1415,15 @@
         <f t="shared" si="0"/>
         <v>237.66666666666666</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>16</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1286,8 +1440,15 @@
         <f t="shared" si="0"/>
         <v>218.66666666666666</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>17</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1304,8 +1465,15 @@
         <f t="shared" si="0"/>
         <v>199</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>18</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1322,8 +1490,15 @@
         <f t="shared" si="0"/>
         <v>189</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>19</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1340,17 +1515,24 @@
         <f t="shared" si="0"/>
         <v>179</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="G24">
+        <v>20</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1367,7 +1549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1385,7 +1567,7 @@
         <v>805.33333333333337</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2.5</v>
       </c>
@@ -1406,7 +1588,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1427,7 +1609,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1448,7 +1630,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1737,13 +1919,13 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -2124,10 +2306,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A49:E49"/>
+    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added pull correct as well as push correct.
</commit_message>
<xml_diff>
--- a/TestData/SensorToWallCmMeasurements.xlsx
+++ b/TestData/SensorToWallCmMeasurements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Sensor to Wall (cm)</t>
   </si>
@@ -44,6 +44,45 @@
   <si>
     <t>FRONT IR SENSOR; After Weird Behavior</t>
   </si>
+  <si>
+    <t>Left Sensor Maximum Dist from Left Wall</t>
+  </si>
+  <si>
+    <t>Right Sensor Maximum Dist from Right Wall</t>
+  </si>
+  <si>
+    <t>&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Left Center</t>
+  </si>
+  <si>
+    <t>Right Center</t>
+  </si>
+  <si>
+    <t>L Off Ctr</t>
+  </si>
+  <si>
+    <t>R Off Ctr</t>
+  </si>
+  <si>
+    <t>4.75 cm from left</t>
+  </si>
+  <si>
+    <t>4.75 cm from right</t>
+  </si>
+  <si>
+    <t>From Edge of Frame to Wall</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>x cm from left</t>
+  </si>
+  <si>
+    <t>x cm from right</t>
+  </si>
 </sst>
 </file>
 
@@ -66,12 +105,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -104,6 +155,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,11 +546,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="144931840"/>
-        <c:axId val="75405504"/>
+        <c:axId val="146237440"/>
+        <c:axId val="97540288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144931840"/>
+        <c:axId val="146237440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +583,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75405504"/>
+        <c:crossAx val="97540288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -538,7 +591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75405504"/>
+        <c:axId val="97540288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -568,7 +621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144931840"/>
+        <c:crossAx val="146237440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -594,16 +647,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>285749</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>61913</xdr:rowOff>
+      <xdr:rowOff>90488</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -912,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,9 +976,13 @@
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="3"/>
     <col min="5" max="5" width="9.140625" style="5"/>
+    <col min="11" max="11" width="6.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -940,8 +997,11 @@
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -972,8 +1032,17 @@
       <c r="K2" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>360</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -998,7 +1067,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1022,8 +1091,11 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.5</v>
       </c>
@@ -1047,8 +1119,17 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>280</v>
+      </c>
+      <c r="N5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1073,7 +1154,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.5</v>
       </c>
@@ -1097,8 +1178,14 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1122,8 +1209,14 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>550</v>
+      </c>
+      <c r="N8">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1148,7 +1241,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1171,9 +1264,20 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1196,9 +1300,20 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="5">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="10">
+        <v>580</v>
+      </c>
+      <c r="N11">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1221,9 +1336,20 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="5">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12">
+        <v>520</v>
+      </c>
+      <c r="N12" s="10">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1246,9 +1372,17 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="5">
+        <v>2</v>
+      </c>
+      <c r="L13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="9">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1271,9 +1405,17 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="5">
+        <v>2</v>
+      </c>
+      <c r="L14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="9">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1298,7 +1440,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Added hardcoded ai functionality so that we can test whether it is reasonable to assume that the mouse will get to the center of the maze with the current autocorrect code. Else, autocorrect is still in progress and a mess as we test many ideas
</commit_message>
<xml_diff>
--- a/TestData/SensorToWallCmMeasurements.xlsx
+++ b/TestData/SensorToWallCmMeasurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="9015"/>
+    <workbookView xWindow="480" yWindow="165" windowWidth="22995" windowHeight="8955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>Sensor to Wall (cm)</t>
   </si>
@@ -82,6 +82,54 @@
   </si>
   <si>
     <t>x cm from right</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>R Sensor Only</t>
+  </si>
+  <si>
+    <t>Between R and S</t>
+  </si>
+  <si>
+    <t>S Sensor Only</t>
+  </si>
+  <si>
+    <t>Between L and S</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Crash Sequence: What does Microtaur see when it has crashed?</t>
+  </si>
+  <si>
+    <t>Closer sensor to wall</t>
+  </si>
+  <si>
+    <t>L Sensor Only</t>
+  </si>
+  <si>
+    <t>Left/Right sensor readouts after a tuple has been detected (worst case)</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Straight</t>
+  </si>
+  <si>
+    <t>(absence of R wall triggers continue_to_center)</t>
+  </si>
+  <si>
+    <t>Event?</t>
   </si>
 </sst>
 </file>
@@ -105,7 +153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +172,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -137,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -152,11 +206,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -206,7 +267,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -546,11 +606,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146237440"/>
-        <c:axId val="97540288"/>
+        <c:axId val="144738304"/>
+        <c:axId val="87578816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146237440"/>
+        <c:axId val="144738304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,14 +636,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97540288"/>
+        <c:crossAx val="87578816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -591,7 +650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97540288"/>
+        <c:axId val="87578816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -614,21 +673,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146237440"/>
+        <c:crossAx val="144738304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -967,7 +1024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -983,20 +1040,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
       <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1306,7 +1363,7 @@
       <c r="L11" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="9">
         <v>580</v>
       </c>
       <c r="N11">
@@ -1345,7 +1402,7 @@
       <c r="M12">
         <v>520</v>
       </c>
-      <c r="N12" s="10">
+      <c r="N12" s="9">
         <v>450</v>
       </c>
     </row>
@@ -1378,7 +1435,7 @@
       <c r="L13" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="8">
         <v>440</v>
       </c>
     </row>
@@ -1411,7 +1468,7 @@
       <c r="L14" t="s">
         <v>21</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="8">
         <v>380</v>
       </c>
     </row>
@@ -1666,13 +1723,13 @@
       <c r="K24" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -2061,13 +2118,13 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -2462,24 +2519,410 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>719</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>708</v>
+      </c>
+      <c r="C4">
+        <v>596</v>
+      </c>
+      <c r="D4">
+        <v>681</v>
+      </c>
+      <c r="F4">
+        <v>130</v>
+      </c>
+      <c r="H4">
+        <v>879</v>
+      </c>
+      <c r="I4">
+        <v>521</v>
+      </c>
+      <c r="K4">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>702</v>
+      </c>
+      <c r="C5">
+        <v>624</v>
+      </c>
+      <c r="D5">
+        <v>790</v>
+      </c>
+      <c r="F5">
+        <v>414</v>
+      </c>
+      <c r="H5">
+        <v>693</v>
+      </c>
+      <c r="I5">
+        <v>582</v>
+      </c>
+      <c r="K5">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>725</v>
+      </c>
+      <c r="C6">
+        <v>609</v>
+      </c>
+      <c r="D6">
+        <v>692</v>
+      </c>
+      <c r="F6">
+        <v>163</v>
+      </c>
+      <c r="H6">
+        <v>739</v>
+      </c>
+      <c r="I6">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>713</v>
+      </c>
+      <c r="F7">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>648</v>
+      </c>
+      <c r="F10">
+        <v>396</v>
+      </c>
+      <c r="G10" s="10">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>738</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11" s="10">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E12" s="10">
+        <v>910</v>
+      </c>
+      <c r="F12">
+        <v>493</v>
+      </c>
+      <c r="G12">
+        <v>983</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>609</v>
+      </c>
+      <c r="B3">
+        <v>494</v>
+      </c>
+      <c r="C3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>626</v>
+      </c>
+      <c r="B4">
+        <v>474</v>
+      </c>
+      <c r="C4">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>681</v>
+      </c>
+      <c r="B5">
+        <v>489</v>
+      </c>
+      <c r="C5">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>602</v>
+      </c>
+      <c r="B6">
+        <v>150</v>
+      </c>
+      <c r="C6">
+        <v>252</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>629</v>
+      </c>
+      <c r="B7">
+        <v>97</v>
+      </c>
+      <c r="C7">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>777</v>
+      </c>
+      <c r="B8">
+        <v>154</v>
+      </c>
+      <c r="C8">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>524</v>
+      </c>
+      <c r="B9">
+        <v>168</v>
+      </c>
+      <c r="C9">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>244</v>
+      </c>
+      <c r="B10">
+        <v>167</v>
+      </c>
+      <c r="C10">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>186</v>
+      </c>
+      <c r="B11">
+        <v>165</v>
+      </c>
+      <c r="C11">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>170</v>
+      </c>
+      <c r="B12">
+        <v>188</v>
+      </c>
+      <c r="C12">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>172</v>
+      </c>
+      <c r="B13">
+        <v>207</v>
+      </c>
+      <c r="C13">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>194</v>
+      </c>
+      <c r="B14">
+        <v>265</v>
+      </c>
+      <c r="C14">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>212</v>
+      </c>
+      <c r="B15">
+        <v>254</v>
+      </c>
+      <c r="C15">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>215</v>
+      </c>
+      <c r="B16">
+        <v>267</v>
+      </c>
+      <c r="C16">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>242</v>
+      </c>
+      <c r="B17">
+        <v>298</v>
+      </c>
+      <c r="C17">
+        <v>455</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hardcoded agent fine tuned. Can reliably get 10 decision points into the maze without error.
</commit_message>
<xml_diff>
--- a/TestData/SensorToWallCmMeasurements.xlsx
+++ b/TestData/SensorToWallCmMeasurements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>Sensor to Wall (cm)</t>
   </si>
@@ -606,11 +606,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="144738304"/>
-        <c:axId val="87578816"/>
+        <c:axId val="149662720"/>
+        <c:axId val="59676864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144738304"/>
+        <c:axId val="149662720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -642,7 +642,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87578816"/>
+        <c:crossAx val="59676864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -650,7 +650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87578816"/>
+        <c:axId val="59676864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144738304"/>
+        <c:crossAx val="149662720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2727,198 +2727,224 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="I2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="J2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="K2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="I3">
+        <v>734</v>
+      </c>
+      <c r="J3">
+        <v>323</v>
+      </c>
+      <c r="K3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>609</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>494</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>626</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>474</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>681</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>489</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>602</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>150</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>252</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>629</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>97</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>777</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>154</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>524</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>168</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>244</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>167</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>186</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>165</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>315</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>170</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>188</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>172</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>207</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>349</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>194</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>265</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>212</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>254</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>412</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>215</v>
-      </c>
-      <c r="B16">
-        <v>267</v>
-      </c>
-      <c r="C16">
-        <v>452</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>215</v>
+      </c>
+      <c r="B17">
+        <v>267</v>
+      </c>
+      <c r="C17">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>242</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>298</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>455</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Micromouse code without delays.
</commit_message>
<xml_diff>
--- a/TestData/SensorToWallCmMeasurements.xlsx
+++ b/TestData/SensorToWallCmMeasurements.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="9015"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="9015" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="IR Sensor to CM Conversion" sheetId="1" r:id="rId1"/>
+    <sheet name="Tuple Recognition Statistics" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Sensor to Wall (cm)</t>
   </si>
@@ -56,12 +56,51 @@
   <si>
     <t>CM</t>
   </si>
+  <si>
+    <t>Tuple Recognition Statistics</t>
+  </si>
+  <si>
+    <t>Units Traveled</t>
+  </si>
+  <si>
+    <t>L clicks</t>
+  </si>
+  <si>
+    <t>R clicks</t>
+  </si>
+  <si>
+    <t>Approx 1 Unit L</t>
+  </si>
+  <si>
+    <t>Approx 1 Unit R</t>
+  </si>
+  <si>
+    <t>Approx 1 Unit Average</t>
+  </si>
+  <si>
+    <t>Outliers L</t>
+  </si>
+  <si>
+    <t>Outliers R</t>
+  </si>
+  <si>
+    <t>&lt;-- started reprogramming after every poll to figure out if debugger is causing the outliers</t>
+  </si>
+  <si>
+    <t>35 clock pulses per 50 ms</t>
+  </si>
+  <si>
+    <t>WE WILL USE TIMER1; TIMER0 DOESN’T WORK!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +111,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -98,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -110,9 +157,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -120,6 +164,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -171,7 +221,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -191,7 +240,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$24</c:f>
+              <c:f>'IR Sensor to CM Conversion'!$A$3:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -266,7 +315,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$24</c:f>
+              <c:f>'IR Sensor to CM Conversion'!$E$3:$E$24</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="22"/>
@@ -352,7 +401,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$28:$E$47</c:f>
+              <c:f>'IR Sensor to CM Conversion'!$E$28:$E$47</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
@@ -432,7 +481,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$51:$E$70</c:f>
+              <c:f>'IR Sensor to CM Conversion'!$E$51:$E$70</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
@@ -511,11 +560,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="48455168"/>
-        <c:axId val="40201600"/>
+        <c:axId val="140806144"/>
+        <c:axId val="40458432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48455168"/>
+        <c:axId val="140806144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,14 +590,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40201600"/>
+        <c:crossAx val="40458432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -556,7 +604,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40201600"/>
+        <c:axId val="40458432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -579,21 +627,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48455168"/>
+        <c:crossAx val="140806144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -932,7 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
@@ -945,13 +991,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1367,13 +1413,13 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1762,13 +1808,13 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -2171,11 +2217,11 @@
       <c r="A74">
         <v>534</v>
       </c>
-      <c r="B74" s="10">
+      <c r="B74" s="9">
         <f>AVERAGE(A74:A79)</f>
         <v>542.66666666666663</v>
       </c>
-      <c r="C74" s="10">
+      <c r="C74" s="9">
         <f>_xlfn.STDEV.P(A74:A79)</f>
         <v>11.86966254317657</v>
       </c>
@@ -2187,87 +2233,87 @@
       <c r="A75">
         <v>531</v>
       </c>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>540</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>551</v>
       </c>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>535</v>
       </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>565</v>
       </c>
-      <c r="B79" s="10"/>
-      <c r="C79" s="10"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B81" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="C81" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="9">
+      <c r="A82" s="8">
         <v>409</v>
       </c>
-      <c r="B82" s="10">
+      <c r="B82" s="9">
         <f>AVERAGE(A82:A87)</f>
         <v>426.5</v>
       </c>
-      <c r="C82" s="10">
+      <c r="C82" s="9">
         <f>_xlfn.STDEV.P(A82:A87)</f>
         <v>15.88238017426859</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="9">
+      <c r="A83" s="8">
         <v>447</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="9">
+      <c r="A84" s="8">
         <v>432</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="9">
+      <c r="A85" s="8">
         <v>418</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="9">
+      <c r="A86" s="8">
         <v>445</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="9">
+      <c r="A87" s="8">
         <v>408</v>
       </c>
     </row>
@@ -2285,13 +2331,472 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>990</v>
+      </c>
+      <c r="D3">
+        <f>C3/A3</f>
+        <v>990</v>
+      </c>
+      <c r="E3">
+        <f>AVERAGE(D3:D16)</f>
+        <v>990.88419913419909</v>
+      </c>
+      <c r="H3">
+        <f>B3/A3</f>
+        <v>21</v>
+      </c>
+      <c r="I3">
+        <f>(H3+D3)/2</f>
+        <v>505.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>998</v>
+      </c>
+      <c r="D4">
+        <f>C4/A4</f>
+        <v>998</v>
+      </c>
+      <c r="H4">
+        <f>B4/A4</f>
+        <v>28</v>
+      </c>
+      <c r="I4">
+        <f>(H4+D4)/2</f>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>1005</v>
+      </c>
+      <c r="D5">
+        <f>C5/A5</f>
+        <v>1005</v>
+      </c>
+      <c r="H5">
+        <f>B5/A5</f>
+        <v>22</v>
+      </c>
+      <c r="I5">
+        <f>(H5+D5)/2</f>
+        <v>513.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1002</v>
+      </c>
+      <c r="C6">
+        <v>1949</v>
+      </c>
+      <c r="D6">
+        <f>C6/A6</f>
+        <v>974.5</v>
+      </c>
+      <c r="H6">
+        <f>B6/A6</f>
+        <v>501</v>
+      </c>
+      <c r="I6">
+        <f>(H6+D6)/2</f>
+        <v>737.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1009</v>
+      </c>
+      <c r="C7">
+        <v>1929</v>
+      </c>
+      <c r="D7">
+        <f>C7/A7</f>
+        <v>964.5</v>
+      </c>
+      <c r="H7">
+        <f>B7/A7</f>
+        <v>504.5</v>
+      </c>
+      <c r="I7">
+        <f>(H7+D7)/2</f>
+        <v>734.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1104</v>
+      </c>
+      <c r="C8">
+        <v>1988</v>
+      </c>
+      <c r="D8">
+        <f>C8/A8</f>
+        <v>994</v>
+      </c>
+      <c r="H8">
+        <f>B8/A8</f>
+        <v>552</v>
+      </c>
+      <c r="I8">
+        <f>(H8+D8)/2</f>
+        <v>773</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>2073</v>
+      </c>
+      <c r="C9">
+        <v>2988</v>
+      </c>
+      <c r="D9">
+        <f>C9/A9</f>
+        <v>996</v>
+      </c>
+      <c r="H9">
+        <f>B9/A9</f>
+        <v>691</v>
+      </c>
+      <c r="I9">
+        <f>(H9+D9)/2</f>
+        <v>843.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>2008</v>
+      </c>
+      <c r="C10">
+        <v>2969</v>
+      </c>
+      <c r="D10">
+        <f>C10/A10</f>
+        <v>989.66666666666663</v>
+      </c>
+      <c r="H10">
+        <f>B10/A10</f>
+        <v>669.33333333333337</v>
+      </c>
+      <c r="I10">
+        <f>(H10+D10)/2</f>
+        <v>829.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>1994</v>
+      </c>
+      <c r="C11">
+        <v>2909</v>
+      </c>
+      <c r="D11">
+        <f>C11/A11</f>
+        <v>969.66666666666663</v>
+      </c>
+      <c r="H11">
+        <f>B11/A11</f>
+        <v>664.66666666666663</v>
+      </c>
+      <c r="I11">
+        <f>(H11+D11)/2</f>
+        <v>817.16666666666663</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>3038</v>
+      </c>
+      <c r="C12">
+        <v>4033</v>
+      </c>
+      <c r="D12">
+        <f>C12/A12</f>
+        <v>1008.25</v>
+      </c>
+      <c r="H12">
+        <f>B12/A12</f>
+        <v>759.5</v>
+      </c>
+      <c r="I12">
+        <f>(H12+D12)/2</f>
+        <v>883.875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>3072</v>
+      </c>
+      <c r="C13">
+        <v>3998</v>
+      </c>
+      <c r="D13">
+        <f>C13/A13</f>
+        <v>999.5</v>
+      </c>
+      <c r="H13">
+        <f>B13/A13</f>
+        <v>768</v>
+      </c>
+      <c r="I13">
+        <f>(H13+D13)/2</f>
+        <v>883.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>3023</v>
+      </c>
+      <c r="C14">
+        <v>4006</v>
+      </c>
+      <c r="D14">
+        <f>C14/A14</f>
+        <v>1001.5</v>
+      </c>
+      <c r="H14">
+        <f>B14/A14</f>
+        <v>755.75</v>
+      </c>
+      <c r="I14">
+        <f>(H14+D14)/2</f>
+        <v>878.625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>3064</v>
+      </c>
+      <c r="C15">
+        <v>3937</v>
+      </c>
+      <c r="D15">
+        <f>C15/A15</f>
+        <v>984.25</v>
+      </c>
+      <c r="H15">
+        <f>B15/A15</f>
+        <v>766</v>
+      </c>
+      <c r="I15">
+        <f>(H15+D15)/2</f>
+        <v>875.125</v>
+      </c>
+      <c r="J15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>10110</v>
+      </c>
+      <c r="C16">
+        <v>10973</v>
+      </c>
+      <c r="D16">
+        <f>C16/A16</f>
+        <v>997.5454545454545</v>
+      </c>
+      <c r="H16">
+        <f>B16/A16</f>
+        <v>919.09090909090912</v>
+      </c>
+      <c r="I16">
+        <f>(H16+D16)/2</f>
+        <v>958.31818181818176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <f>C17/A17</f>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f>B17/A17</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f>(H17+D17)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <f>C18/A18</f>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f>B18/A18</f>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f>(H18+D18)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <f>C19/A19</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f>B19/A19</f>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f>(H19+D19)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <f>C20/A20</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f>B20/A20</f>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f>(H20+D20)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>